<commit_message>
New data, GLEON poster
</commit_message>
<xml_diff>
--- a/data/raw_data/Summer Experiment 2021.xlsx
+++ b/data/raw_data/Summer Experiment 2021.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10808"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10912"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abigaillewis/Desktop/FeDOC/data/raw_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9778200B-BED8-FE47-8850-9470CC7E21C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8441D32D-3DFB-BB40-8BF6-AC8614BB4570}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16260" activeTab="1" xr2:uid="{D690C64F-524F-5D42-BE11-8FEB808CB86F}"/>
   </bookViews>
@@ -877,8 +877,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F96D5079-A55D-3242-9087-7E5A1EDF769D}">
   <dimension ref="A1:M103"/>
   <sheetViews>
-    <sheetView topLeftCell="A85" workbookViewId="0">
-      <selection activeCell="G99" sqref="G99:L103"/>
+    <sheetView topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="E48" sqref="E48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2464,7 +2464,7 @@
         <v>16.100000000000001</v>
       </c>
       <c r="E42">
-        <v>7.13</v>
+        <v>7.1</v>
       </c>
       <c r="F42">
         <v>71.7</v>
@@ -2502,7 +2502,7 @@
         <v>16</v>
       </c>
       <c r="E43">
-        <v>0.01</v>
+        <v>7.13</v>
       </c>
       <c r="F43">
         <v>71.900000000000006</v>
@@ -2540,7 +2540,7 @@
         <v>21.9</v>
       </c>
       <c r="E44">
-        <v>0.02</v>
+        <v>0.01</v>
       </c>
       <c r="F44">
         <v>0.2</v>
@@ -4815,8 +4815,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{065DBBA8-3A56-F045-BC1F-26589A180D06}">
   <dimension ref="A1:K103"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
-      <selection activeCell="H109" sqref="H109"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="E50" sqref="E50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>